<commit_message>
Delete Userdefined group testcases
</commit_message>
<xml_diff>
--- a/AndroidAutomation_Farmer/src/main/resources/TestData_FarmerAPK.xlsx
+++ b/AndroidAutomation_Farmer/src/main/resources/TestData_FarmerAPK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15585" windowHeight="4065" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15585" windowHeight="4065" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterCattle" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ForgotPin" sheetId="11" r:id="rId11"/>
     <sheet name="CreateUserdefinedshed" sheetId="13" r:id="rId12"/>
     <sheet name="AddCattletoUserdefinedShed" sheetId="14" r:id="rId13"/>
+    <sheet name="DeleteUserdefinedGroup" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="240">
   <si>
     <t>testcase</t>
   </si>
@@ -727,6 +728,39 @@
   </si>
   <si>
     <t>Deselect all the selected cattle to add cattle to group</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete the Group grp_No from Shed shed_No?</t>
+  </si>
+  <si>
+    <t>Group grp_No is the last group in the Shed shed_No. Deleting this Group grp_No will also delete the Shed shed_No. Do you want to proceed?</t>
+  </si>
+  <si>
+    <t>successMessage</t>
+  </si>
+  <si>
+    <t>DeleteUserdefinedGroup_deleteGrp</t>
+  </si>
+  <si>
+    <t>DeleteUserdefinedGroup_deletelastGrp</t>
+  </si>
+  <si>
+    <t>DeleteUserdefinedGroup_deleteGrpwithCattle</t>
+  </si>
+  <si>
+    <t>Move all cattle out from this group</t>
+  </si>
+  <si>
+    <t>Group - grp_No has been deleted from Shed shed_No.</t>
+  </si>
+  <si>
+    <t>Group grp_No is the last group in the last active Shed shed_No. Deleting this Group grp_No will delete all Sheds and Groups in Housing and will Reset Housing. Do you want to proceed?</t>
+  </si>
+  <si>
+    <t>DeleteUserdefinedGroup_deletelastGrpoflastShed</t>
+  </si>
+  <si>
+    <t>All cattle been moved out from Group grp_No</t>
   </si>
 </sst>
 </file>
@@ -814,7 +848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -830,6 +864,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1138,7 +1175,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1827,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,6 +1912,78 @@
       </c>
       <c r="B5" t="s">
         <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete Userdefined Shed Testcases and upload Photo functions
</commit_message>
<xml_diff>
--- a/AndroidAutomation_Farmer/src/main/resources/TestData_FarmerAPK.xlsx
+++ b/AndroidAutomation_Farmer/src/main/resources/TestData_FarmerAPK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15585" windowHeight="4065" firstSheet="10" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14685" windowHeight="5610" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterCattle" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="CreateUserdefinedshed" sheetId="13" r:id="rId12"/>
     <sheet name="AddCattletoUserdefinedShed" sheetId="14" r:id="rId13"/>
     <sheet name="DeleteUserdefinedGroup" sheetId="15" r:id="rId14"/>
+    <sheet name="DeleteUserdefinedShed" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="242">
   <si>
     <t>testcase</t>
   </si>
@@ -761,6 +762,12 @@
   </si>
   <si>
     <t>All cattle been moved out from Group grp_No</t>
+  </si>
+  <si>
+    <t>All Groups in Shed must be deleted in order to delete the Shed</t>
+  </si>
+  <si>
+    <t>DeleteUserdefinedShed_withoutDeletingNonEmptyGroups</t>
   </si>
 </sst>
 </file>
@@ -848,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -869,6 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,6 +1992,41 @@
       </c>
       <c r="C5" t="s">
         <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>